<commit_message>
Sea enxa el procedimiento almacenado spCBConciliarPedidosPorReferenciaPorMovExterno
</commit_message>
<xml_diff>
--- a/Documentos/FormaConciliacion.xlsx
+++ b/Documentos/FormaConciliacion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="180">
   <si>
     <t>CONCILIACION DE EGRESOS</t>
   </si>
@@ -598,6 +598,12 @@
   </si>
   <si>
     <t>Fecha compromiso</t>
+  </si>
+  <si>
+    <t>6.1.5</t>
+  </si>
+  <si>
+    <t>Jorge-1</t>
   </si>
 </sst>
 </file>
@@ -1140,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="K1:M1"/>
+    <sheetView topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,7 +1915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="C17" t="s">
         <v>78</v>
@@ -1918,19 +1924,25 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="C18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>179</v>
+      </c>
+      <c r="J18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="C19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>96</v>
       </c>
@@ -1941,13 +1953,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="C21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="C22" t="s">
         <v>90</v>
@@ -1956,18 +1968,18 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="C23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>99</v>
       </c>
@@ -1975,38 +1987,38 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="C31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="C32" t="s">
         <v>84</v>

</xml_diff>